<commit_message>
学习并总结了英语的16种时态：https://blog.csdn.net/namelessmyth/article/details/134161822?spm=1001.2014.3001.5501 视频《MySQL实战调优》看了25~34，约2小时。个别章节没听懂，明天重新听一下。 导入MySQL官网的sakila-db脚本。Dbeaver用不习惯，安装了Navicat Premium 16.1.15
</commit_message>
<xml_diff>
--- a/report/周期报告-2023-Gem.xlsx
+++ b/report/周期报告-2023-Gem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\resource\git-doc\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FC49B7-64AA-4258-BDC0-1DE52E05CBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D319CDA6-9BF8-4A0B-A92F-F55A3382DB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="409">
   <si>
     <t>汇报日期</t>
   </si>
@@ -2314,37 +2314,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1.延期完成。8:55计划，23:05日报
-2.未完成。
-3.完成。20:00~21:30，2题
-4.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>未完成</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>。
-5.完成。74.9kg，晚上吃了栗子</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.完成。实际：5天
 2.完成。实际：mongoDB，11题
 3.完成。实际：已完成
@@ -2372,14 +2341,6 @@
   </si>
   <si>
     <t>上午学习英语article10，晚上写了周报和leetcode题目。1321. 餐馆营业额变化增长。602. 好友申请 II ：谁有最多的好友。学到了高级SQL语法over(order by date range interval 6 day preceding),写了Mermaid笔记。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.完成。7:55计划，22:56日报
-2.完成。09:30~10:30，article10
-3.完成。22:00~22:50，2题
-4.完成。
-5.完成。75.7kg，晚上吃了栗子</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2422,6 +2383,48 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1.7点起床做计划，23点日报睡觉
+2.英语, 学习3小时
+3.leetcode，2题
+4.mysql视频3小时
+5.体重减到75.3kg(非必须)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最近5天，状态下滑，没有完成当日目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主观原因：执行力不足，虽然有客观原因。但主观上自控力还是不足。容易受干扰。
+主观原因：出现干扰因素之后，没有及时调整反而因此觉得目标不完成也有理由了。
+客观原因：周末家人生病需要去医院并照顾，周一有朋友有事需要帮忙。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>心得总结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出现任务偏差后，要有奖惩措施，仅仅写检讨是不够的。这个检讨措施最好是自己在乎的，但是又不会影响整体计划太多的。本次奖惩措施。今天目标如果不完成，不允许去淘宝购物，直到某天的任务完成才能去购物。如果本周目标不完成或者可能完不成，淘宝只允许买300以内必须商品。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.7点起床做计划，23点日报睡觉
+2.英语, 学习3小时
+3.leetcode，2题
+4.mysql视频3小时
+5.体重减到75.2kg(非必须)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.完成。7:47计划，23:35日报
+2.完成。09:47~15:00，3小时
+3.完成。16:00~17:30，2题
+4.完成。17:45~23:00，3小时
+5.完成。75.0kg，中晚饭代餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>1.完成。7:38计划，23:05日报
 2.完成。09:20~13:00，3小时
@@ -2448,42 +2451,47 @@
         <charset val="134"/>
       </rPr>
       <t>。19:00~23:50，1小时
-5.完成。75.5kg，晚上吃了栗子</t>
+5.完成。75.5kg，</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.7点起床做计划，23点日报睡觉
-2.英语, 学习3小时
-3.leetcode，2题
-4.mysql视频3小时
-5.体重减到75.3kg(非必须)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最近5天，状态下滑，没有完成当日目标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主观原因：执行力不足，虽然有客观原因。但主观上自控力还是不足。容易受干扰。
-主观原因：出现干扰因素之后，没有及时调整反而因此觉得目标不完成也有理由了。
-客观原因：周末家人生病需要去医院并照顾，周一有朋友有事需要帮忙。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>心得总结</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出现任务偏差后，要有奖惩措施，仅仅写检讨是不够的。这个检讨措施最好是自己在乎的，但是又不会影响整体计划太多的。本次奖惩措施。今天目标如果不完成，不允许去淘宝购物，直到某天的任务完成才能去购物。如果本周目标不完成或者可能完不成，淘宝只允许买300以内必须商品。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.完成。7:47计划，23:05日报
-2.完成。09:47~15:00，3小时
-3.完成。16:00~17:30，2题
-4.完成。17:45~23:00，3小时
-5.完成。74.9kg，晚上吃了栗子</t>
+    <t>1.完成。7:55计划，22:56日报
+2.完成。09:30~10:30，article10
+3.完成。22:00~22:50，2题
+4.完成。
+5.完成。75.7kg，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.延期完成。8:55计划，23:05日报
+2.未完成。
+3.完成。20:00~21:30，2题
+4.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>未完成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。
+5.完成。74.9kg，</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2491,11 +2499,73 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.7点起床做计划，23点日报睡觉
-2.英语, 学习3小时
-3.leetcode，2题
-4.mysql视频3小时
-5.体重减到75.2kg(非必须)</t>
+    <t>英语：用表格和甘特图整理了英语的16种时态。同时整理并复习了mermaid的甘特图语法。leetcode:1527. 患某种疾病的患者, 196. 删除重复的电子邮箱.学习到了一个删除表中重复数据的好办法。导入MySQL官网的sakila-db脚本。Dbeaver用不习惯，安装了Navicat Premium 16.1.15。视频《MySQL实战调优》看了25~34，约2小时。个别章节没听懂，明天重新听一下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.完成。7:40计划，23:05日报，检讨
+2.完成。09:45~15:30，5小时
+3.完成。15:30~16:00，2题
+4.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>未完成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。17:00~23:59，2小时
+5.完成。74.9kg，中晚饭代餐</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.延期完成。7:40计划，00:15日报
+2.完成。09:45~15:30，5小时
+3.完成。15:30~16:00，2题
+4.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>未完成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。17:00~23:59，2小时
+5.完成。74.9kg，中晚饭代餐</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:20之前出门，去自习室。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2775,7 +2845,49 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="240">
+  <dxfs count="244">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -5667,10 +5779,10 @@
         <v>45235</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="31"/>
@@ -5708,10 +5820,10 @@
         <v>361</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>387</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>388</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="1"/>
@@ -7222,16 +7334,16 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B64:B1048576 B8:B53 B1">
-    <cfRule type="cellIs" dxfId="239" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="91" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="92" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="93" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="95" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="96">
@@ -7246,16 +7358,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="235" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="86" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="87" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="88" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="89" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="90">
@@ -7270,16 +7382,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="231" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="81" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="82" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="83" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="84" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="85">
@@ -7294,16 +7406,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="cellIs" dxfId="227" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="76" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="77" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="78" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="79" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="80">
@@ -7318,16 +7430,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="cellIs" dxfId="223" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="71" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="72" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="73" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="74" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="75">
@@ -7342,16 +7454,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="cellIs" dxfId="219" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="66" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="67" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="68" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="69" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="70">
@@ -7366,16 +7478,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="215" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="61" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="62" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="63" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="64" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="65">
@@ -7390,16 +7502,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="cellIs" dxfId="211" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="56" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="57" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="58" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="59" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="60">
@@ -7414,16 +7526,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="207" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="51" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="52" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="53" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="54" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="55">
@@ -7438,16 +7550,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="cellIs" dxfId="203" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="46" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="47" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="48" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="49" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="50">
@@ -7462,16 +7574,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="cellIs" dxfId="199" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="36" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="37" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="38" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="39" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="40">
@@ -7486,16 +7598,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="cellIs" dxfId="195" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="31" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="32" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="33" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="34" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="35">
@@ -7510,16 +7622,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="cellIs" dxfId="191" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="26" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="27" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="28" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="29" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="30">
@@ -7534,16 +7646,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="187" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="21" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="22" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="23" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="24" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="25">
@@ -7558,16 +7670,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="183" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="16" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="17" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="18" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="19" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="20">
@@ -7582,16 +7694,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="179" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="6" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="8" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="9" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -7606,16 +7718,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="175" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="1" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="2" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="3" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="4" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -7642,7 +7754,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W70"/>
+  <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -7701,21 +7813,21 @@
     </row>
     <row r="2" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
-        <v>45231</v>
+        <v>45232</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>301</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="10" t="s">
-        <v>134</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>408</v>
+      </c>
+      <c r="F2" s="10"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -7736,19 +7848,19 @@
     </row>
     <row r="3" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
-        <v>45230</v>
+        <v>45231</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>135</v>
@@ -7773,19 +7885,19 @@
     </row>
     <row r="4" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
-        <v>45229</v>
+        <v>45230</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>135</v>
@@ -7810,19 +7922,19 @@
     </row>
     <row r="5" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
-        <v>45228</v>
+        <v>45229</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>135</v>
@@ -7847,19 +7959,19 @@
     </row>
     <row r="6" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
-        <v>45227</v>
+        <v>45228</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>386</v>
+        <v>402</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>135</v>
@@ -7884,19 +7996,19 @@
     </row>
     <row r="7" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
-        <v>45226</v>
+        <v>45227</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>135</v>
@@ -7921,19 +8033,19 @@
     </row>
     <row r="8" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
-        <v>45225</v>
+        <v>45226</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>135</v>
@@ -7958,22 +8070,22 @@
     </row>
     <row r="9" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
-        <v>45224</v>
+        <v>45225</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -7995,22 +8107,22 @@
     </row>
     <row r="10" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
-        <v>45223</v>
+        <v>45224</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -8032,19 +8144,19 @@
     </row>
     <row r="11" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
-        <v>45222</v>
+        <v>45223</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>366</v>
+        <v>375</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>373</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>135</v>
@@ -8069,19 +8181,19 @@
     </row>
     <row r="12" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
-        <v>45221</v>
+        <v>45222</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>135</v>
@@ -8106,22 +8218,22 @@
     </row>
     <row r="13" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -8143,22 +8255,22 @@
     </row>
     <row r="14" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
-        <v>45219</v>
+        <v>45220</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -8180,19 +8292,19 @@
     </row>
     <row r="15" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
-        <v>45218</v>
+        <v>45219</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>135</v>
@@ -8217,19 +8329,19 @@
     </row>
     <row r="16" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
-        <v>45217</v>
+        <v>45218</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>135</v>
@@ -8252,24 +8364,24 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="74.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
-        <v>45216</v>
+        <v>45217</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -8291,22 +8403,22 @@
     </row>
     <row r="18" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
-        <v>45215</v>
+        <v>45216</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>341</v>
+        <v>371</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -8328,19 +8440,19 @@
     </row>
     <row r="19" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
-        <v>45213</v>
+        <v>45215</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>135</v>
@@ -8365,19 +8477,19 @@
     </row>
     <row r="20" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
-        <v>45212</v>
+        <v>45213</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>135</v>
@@ -8402,19 +8514,19 @@
     </row>
     <row r="21" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
-        <v>45211</v>
+        <v>45212</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>135</v>
@@ -8439,19 +8551,19 @@
     </row>
     <row r="22" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
-        <v>45210</v>
+        <v>45211</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>135</v>
@@ -8476,19 +8588,19 @@
     </row>
     <row r="23" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A23" s="28">
-        <v>45209</v>
+        <v>45210</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>135</v>
@@ -8511,21 +8623,21 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
     </row>
-    <row r="24" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A24" s="28">
-        <v>45208</v>
+        <v>45209</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>135</v>
@@ -8548,24 +8660,24 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
     </row>
-    <row r="25" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28">
-        <v>45207</v>
+        <v>45208</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -8587,19 +8699,19 @@
     </row>
     <row r="26" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A26" s="28">
-        <v>45206</v>
+        <v>45207</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>134</v>
@@ -8624,22 +8736,22 @@
     </row>
     <row r="27" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A27" s="28">
-        <v>45205</v>
+        <v>45206</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -8661,19 +8773,19 @@
     </row>
     <row r="28" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A28" s="28">
-        <v>45204</v>
+        <v>45205</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>135</v>
@@ -8696,21 +8808,21 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A29" s="28">
-        <v>45203</v>
+        <v>45204</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>135</v>
@@ -8733,21 +8845,21 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
     </row>
-    <row r="30" spans="1:23" ht="58" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
       <c r="A30" s="28">
-        <v>45199</v>
+        <v>45203</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>135</v>
@@ -8770,24 +8882,24 @@
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
     </row>
-    <row r="31" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="58" x14ac:dyDescent="0.3">
       <c r="A31" s="28">
-        <v>45198</v>
+        <v>45199</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -8807,24 +8919,24 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
     </row>
-    <row r="32" spans="1:23" ht="76.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
       <c r="A32" s="28">
-        <v>45197</v>
+        <v>45198</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -8846,19 +8958,19 @@
     </row>
     <row r="33" spans="1:23" ht="76.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28">
-        <v>45196</v>
+        <v>45197</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>135</v>
@@ -8883,19 +8995,19 @@
     </row>
     <row r="34" spans="1:23" ht="76.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="28">
-        <v>45195</v>
+        <v>45196</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>135</v>
@@ -8918,21 +9030,21 @@
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
     </row>
-    <row r="35" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" ht="76.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28">
-        <v>45194</v>
+        <v>45195</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>257</v>
+        <v>287</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>135</v>
@@ -8955,21 +9067,21 @@
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
     </row>
-    <row r="36" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28">
-        <v>45193</v>
+        <v>45194</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>135</v>
@@ -8992,24 +9104,24 @@
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="28">
-        <v>45192</v>
+        <v>45193</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -9031,22 +9143,22 @@
     </row>
     <row r="38" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="28">
-        <v>45191</v>
+        <v>45192</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -9068,19 +9180,19 @@
     </row>
     <row r="39" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28">
-        <v>45190</v>
+        <v>45191</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>135</v>
@@ -9105,19 +9217,19 @@
     </row>
     <row r="40" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="28">
-        <v>45189</v>
+        <v>45190</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>135</v>
@@ -9142,19 +9254,19 @@
     </row>
     <row r="41" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="28">
-        <v>45188</v>
+        <v>45189</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>135</v>
@@ -9179,19 +9291,19 @@
     </row>
     <row r="42" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="28">
-        <v>45187</v>
+        <v>45188</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>135</v>
@@ -9214,21 +9326,21 @@
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" ht="29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" ht="59" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="28">
-        <v>45186</v>
+        <v>45187</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>135</v>
@@ -9251,21 +9363,21 @@
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="29" x14ac:dyDescent="0.3">
       <c r="A44" s="28">
-        <v>45185</v>
+        <v>45186</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>135</v>
@@ -9290,19 +9402,19 @@
     </row>
     <row r="45" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="28">
-        <v>45184</v>
+        <v>45185</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>135</v>
@@ -9327,19 +9439,19 @@
     </row>
     <row r="46" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="28">
-        <v>45183</v>
+        <v>45184</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>137</v>
+        <v>214</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>139</v>
+        <v>228</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>135</v>
@@ -9364,19 +9476,19 @@
     </row>
     <row r="47" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="28">
-        <v>45182</v>
-      </c>
-      <c r="B47" s="11" t="s">
+        <v>45183</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>135</v>
@@ -9401,7 +9513,7 @@
     </row>
     <row r="48" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="28">
-        <v>45181</v>
+        <v>45182</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>9</v>
@@ -9413,7 +9525,7 @@
         <v>141</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>135</v>
@@ -9438,22 +9550,22 @@
     </row>
     <row r="49" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="28">
-        <v>45180</v>
+        <v>45181</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>140</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -9474,22 +9586,22 @@
       <c r="W49" s="1"/>
     </row>
     <row r="50" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="29">
-        <v>45179</v>
+      <c r="A50" s="28">
+        <v>45180</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D50" s="13" t="s">
+      <c r="C50" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="F50" s="14" t="s">
+      <c r="E50" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50" s="10" t="s">
         <v>134</v>
       </c>
       <c r="G50" s="1"/>
@@ -9511,22 +9623,22 @@
       <c r="W50" s="1"/>
     </row>
     <row r="51" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="28">
-        <v>45178</v>
+      <c r="A51" s="29">
+        <v>45179</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="F51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F51" s="14" t="s">
         <v>134</v>
       </c>
       <c r="G51" s="1"/>
@@ -9549,22 +9661,22 @@
     </row>
     <row r="52" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="28">
-        <v>45176</v>
+        <v>45178</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>135</v>
+        <v>150</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -9586,7 +9698,7 @@
     </row>
     <row r="53" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="28">
-        <v>45175</v>
+        <v>45176</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>9</v>
@@ -9598,7 +9710,7 @@
         <v>141</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>233</v>
+        <v>152</v>
       </c>
       <c r="F53" s="14" t="s">
         <v>135</v>
@@ -9623,21 +9735,23 @@
     </row>
     <row r="54" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="28">
-        <v>45174</v>
+        <v>45175</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F54" s="14"/>
+        <v>233</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -9658,19 +9772,19 @@
     </row>
     <row r="55" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="28">
-        <v>45173</v>
+        <v>45174</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F55" s="14"/>
       <c r="G55" s="1"/>
@@ -9693,7 +9807,7 @@
     </row>
     <row r="56" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="28">
-        <v>45170</v>
+        <v>45173</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>9</v>
@@ -9702,10 +9816,10 @@
         <v>151</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="1"/>
@@ -9728,7 +9842,7 @@
     </row>
     <row r="57" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="28">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>9</v>
@@ -9737,10 +9851,10 @@
         <v>151</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="1"/>
@@ -9762,20 +9876,20 @@
       <c r="W57" s="1"/>
     </row>
     <row r="58" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="29">
-        <v>45168</v>
+      <c r="A58" s="28">
+        <v>45169</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>163</v>
+        <v>9</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>160</v>
       </c>
       <c r="F58" s="14"/>
       <c r="G58" s="1"/>
@@ -9796,21 +9910,21 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="59" spans="1:23" ht="29" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
-        <v>44998</v>
+        <v>45168</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F59" s="14"/>
       <c r="G59" s="1"/>
@@ -9833,19 +9947,19 @@
     </row>
     <row r="60" spans="1:23" ht="29" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
-        <v>44997</v>
+        <v>44998</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F60" s="14"/>
       <c r="G60" s="1"/>
@@ -9868,18 +9982,20 @@
     </row>
     <row r="61" spans="1:23" ht="29" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
-        <v>44995</v>
+        <v>44997</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="E61" s="15"/>
+        <v>168</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>169</v>
+      </c>
       <c r="F61" s="14"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -9901,20 +10017,18 @@
     </row>
     <row r="62" spans="1:23" ht="29" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
-        <v>44994</v>
+        <v>44995</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>164</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>171</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="E62" s="15"/>
       <c r="F62" s="14"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -9936,19 +10050,19 @@
     </row>
     <row r="63" spans="1:23" ht="29" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F63" s="14"/>
       <c r="G63" s="1"/>
@@ -9969,21 +10083,21 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
     </row>
-    <row r="64" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" ht="29" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="1"/>
@@ -10006,19 +10120,19 @@
     </row>
     <row r="65" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="1"/>
@@ -10039,21 +10153,21 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
     </row>
-    <row r="66" spans="1:23" ht="58" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
-        <v>44990</v>
+        <v>44991</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="1"/>
@@ -10074,21 +10188,21 @@
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
     </row>
-    <row r="67" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" ht="58" x14ac:dyDescent="0.3">
       <c r="A67" s="29">
-        <v>44989</v>
+        <v>44990</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F67" s="14"/>
       <c r="G67" s="1"/>
@@ -10111,19 +10225,19 @@
     </row>
     <row r="68" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
-        <v>44988</v>
+        <v>44989</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F68" s="14"/>
       <c r="G68" s="1"/>
@@ -10144,21 +10258,21 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
     </row>
-    <row r="69" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" ht="43.5" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
-        <v>44987</v>
+        <v>44988</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F69" s="14"/>
       <c r="G69" s="1"/>
@@ -10179,21 +10293,21 @@
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
     </row>
-    <row r="70" spans="1:23" ht="58" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A70" s="29">
-        <v>44986</v>
+        <v>44987</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="1"/>
@@ -10214,9 +10328,68 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
+    <row r="71" spans="1:23" ht="58" x14ac:dyDescent="0.3">
+      <c r="A71" s="29">
+        <v>44986</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B44:B1048576 B1">
+  <conditionalFormatting sqref="B45:B1048576 B1">
+    <cfRule type="cellIs" dxfId="175" priority="226" operator="equal">
+      <formula>"部分完成"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="227" operator="equal">
+      <formula>"里程碑"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="228" operator="equal">
+      <formula>"进行中"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="229" operator="equal">
+      <formula>"已完成"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="230">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
     <cfRule type="cellIs" dxfId="171" priority="221" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
@@ -10240,7 +10413,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
+  <conditionalFormatting sqref="B44">
     <cfRule type="cellIs" dxfId="167" priority="216" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
@@ -10264,7 +10437,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43">
+  <conditionalFormatting sqref="B42">
     <cfRule type="cellIs" dxfId="163" priority="211" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
@@ -10361,19 +10534,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="147" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="186" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="187" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="188" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="189" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="195">
+    <cfRule type="colorScale" priority="190">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10409,19 +10582,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="139" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="171" operator="equal">
       <formula>"部分完成"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="172" operator="equal">
       <formula>"里程碑"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="173" operator="equal">
       <formula>"进行中"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="174" operator="equal">
       <formula>"已完成"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="180">
+    <cfRule type="colorScale" priority="175">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11249,7 +11422,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B70" xr:uid="{E6A77140-D970-4A0E-A056-7CC50B06531A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B71" xr:uid="{E6A77140-D970-4A0E-A056-7CC50B06531A}">
       <formula1>"已完成,进行中,部分完成,里程碑,未完成,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -11304,7 +11477,7 @@
         <v>197</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.3">
@@ -11438,13 +11611,13 @@
         <v>301</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>398</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>399</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>